<commit_message>
quase duas da manhã
</commit_message>
<xml_diff>
--- a/dados iypt.xlsx
+++ b/dados iypt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7a01b2c0ff13c9a/Área de Trabalho/flado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{F6231C8F-1D41-484E-A66F-A44FC3D65B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8347DA26-7920-4A5A-99EE-50CA90850D1F}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{F6231C8F-1D41-484E-A66F-A44FC3D65B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9CD822A-FAFA-46EC-A7CC-A90D15C1B976}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA78291E-974B-4465-8370-FB667613188C}"/>
   </bookViews>
@@ -189,7 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -232,6 +232,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1265,16 +1268,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>157162</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>471487</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>461962</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1602,7 +1605,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,15 +1663,15 @@
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="K2" s="16"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="11"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -1692,15 +1695,15 @@
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>4</v>
       </c>
+      <c r="K3" s="17"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -1724,15 +1727,15 @@
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="K4" s="17"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -1756,15 +1759,15 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="K5" s="17"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
@@ -1788,15 +1791,15 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>2</v>
       </c>
+      <c r="K6" s="18"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="11"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3">

</xml_diff>

<commit_message>
espero q esteja acabando
</commit_message>
<xml_diff>
--- a/dados iypt.xlsx
+++ b/dados iypt.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maviv\flado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7a01b2c0ff13c9a/Área de Trabalho/flado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444714E3-998C-464D-83CF-A27F7BD79559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{444714E3-998C-464D-83CF-A27F7BD79559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD8A7D12-3F8E-4D9A-A1E4-788C161F6985}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA78291E-974B-4465-8370-FB667613188C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA78291E-974B-4465-8370-FB667613188C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -2632,21 +2632,21 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="16"/>
-    <col min="2" max="2" width="8.88671875" style="16"/>
-    <col min="3" max="3" width="9.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.88671875" style="17"/>
-    <col min="7" max="8" width="9.109375" style="17"/>
-    <col min="9" max="9" width="8.88671875" style="17"/>
-    <col min="11" max="13" width="9.109375" style="17"/>
+    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="2" max="2" width="8.85546875" style="16"/>
+    <col min="3" max="3" width="9.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.85546875" style="17"/>
+    <col min="7" max="8" width="9.140625" style="17"/>
+    <col min="9" max="9" width="8.85546875" style="17"/>
+    <col min="11" max="13" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10">
         <v>0.3</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="I1" s="12">
-        <f>AVERAGE(G1:H1)</f>
+        <f t="shared" ref="I1:I23" si="0">AVERAGE(G1:H1)</f>
         <v>4.53E-2</v>
       </c>
       <c r="K1" s="13"/>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>0.4</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>2.3099999999999999E-2</v>
       </c>
       <c r="I2" s="12">
-        <f>AVERAGE(G2:H2)</f>
+        <f t="shared" si="0"/>
         <v>3.0600000000000002E-2</v>
       </c>
       <c r="K2" s="13"/>
@@ -2717,7 +2717,7 @@
       <c r="U2" s="3"/>
       <c r="V2" s="4"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>0.5</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="I3" s="12">
-        <f>AVERAGE(G3:H3)</f>
+        <f t="shared" si="0"/>
         <v>3.8449999999999998E-2</v>
       </c>
       <c r="K3" s="13"/>
@@ -2756,7 +2756,7 @@
       <c r="U3" s="6"/>
       <c r="V3" s="7"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>0.6</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>2.1899999999999999E-2</v>
       </c>
       <c r="I4" s="12">
-        <f>AVERAGE(G4:H4)</f>
+        <f t="shared" si="0"/>
         <v>2.4399999999999998E-2</v>
       </c>
       <c r="K4" s="13"/>
@@ -2795,7 +2795,7 @@
       <c r="U4" s="6"/>
       <c r="V4" s="7"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>0.7</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>4.9400000000000006E-2</v>
       </c>
       <c r="I5" s="12">
-        <f>AVERAGE(G5:H5)</f>
+        <f t="shared" si="0"/>
         <v>4.7200000000000006E-2</v>
       </c>
       <c r="K5" s="13"/>
@@ -2834,7 +2834,7 @@
       <c r="U5" s="6"/>
       <c r="V5" s="7"/>
     </row>
-    <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>0.8</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>0.1956</v>
       </c>
       <c r="I6" s="12">
-        <f>AVERAGE(G6:H6)</f>
+        <f t="shared" si="0"/>
         <v>0.14030000000000001</v>
       </c>
       <c r="K6" s="13"/>
@@ -2873,7 +2873,7 @@
       <c r="U6" s="6"/>
       <c r="V6" s="7"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>0.9</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>0.16120000000000001</v>
       </c>
       <c r="I7" s="12">
-        <f>AVERAGE(G7:H7)</f>
+        <f t="shared" si="0"/>
         <v>0.1956</v>
       </c>
       <c r="K7" s="13"/>
@@ -2911,7 +2911,7 @@
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>1</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>0.24690000000000001</v>
       </c>
       <c r="I8" s="12">
-        <f>AVERAGE(G8:H8)</f>
+        <f t="shared" si="0"/>
         <v>0.23535</v>
       </c>
       <c r="K8" s="13"/>
@@ -2949,7 +2949,7 @@
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1.1000000000000001</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>0.1875</v>
       </c>
       <c r="I9" s="12">
-        <f>AVERAGE(G9:H9)</f>
+        <f t="shared" si="0"/>
         <v>0.21279999999999999</v>
       </c>
       <c r="K9" s="13"/>
@@ -2987,7 +2987,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>1.2</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>0.29620000000000002</v>
       </c>
       <c r="I10" s="12">
-        <f>AVERAGE(G10:H10)</f>
+        <f t="shared" si="0"/>
         <v>0.27655000000000002</v>
       </c>
       <c r="K10" s="13"/>
@@ -3025,7 +3025,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>1.3</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>0.3906</v>
       </c>
       <c r="I11" s="12">
-        <f>AVERAGE(G11:H11)</f>
+        <f t="shared" si="0"/>
         <v>0.39560000000000001</v>
       </c>
       <c r="K11" s="13"/>
@@ -3063,7 +3063,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>1.4</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>0.42749999999999999</v>
       </c>
       <c r="I12" s="12">
-        <f>AVERAGE(G12:H12)</f>
+        <f t="shared" si="0"/>
         <v>0.41565000000000002</v>
       </c>
       <c r="K12" s="13"/>
@@ -3101,7 +3101,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>1.5</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>0.42810000000000004</v>
       </c>
       <c r="I13" s="12">
-        <f>AVERAGE(G13:H13)</f>
+        <f t="shared" si="0"/>
         <v>0.45905000000000001</v>
       </c>
       <c r="K13" s="13"/>
@@ -3132,7 +3132,7 @@
         <v>0.43406250000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1.6</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>0.5675</v>
       </c>
       <c r="I14" s="12">
-        <f>AVERAGE(G14:H14)</f>
+        <f t="shared" si="0"/>
         <v>0.54249999999999998</v>
       </c>
       <c r="K14" s="13"/>
@@ -3163,7 +3163,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>1.7</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>0.57810000000000006</v>
       </c>
       <c r="I15" s="12">
-        <f>AVERAGE(G15:H15)</f>
+        <f t="shared" si="0"/>
         <v>0.57935000000000003</v>
       </c>
       <c r="K15" s="13"/>
@@ -3194,7 +3194,7 @@
         <v>0.56468750000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1.8</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>0.56559999999999999</v>
       </c>
       <c r="I16" s="12">
-        <f>AVERAGE(G16:H16)</f>
+        <f t="shared" si="0"/>
         <v>0.57155</v>
       </c>
       <c r="K16" s="13"/>
@@ -3228,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>1.9</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>0.70120000000000005</v>
       </c>
       <c r="I17" s="12">
-        <f>AVERAGE(G17:H17)</f>
+        <f t="shared" si="0"/>
         <v>0.70965000000000011</v>
       </c>
       <c r="K17" s="13"/>
@@ -3259,7 +3259,7 @@
         <v>0.70843750000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>2</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>0.72689999999999999</v>
       </c>
       <c r="I18" s="12">
-        <f>AVERAGE(G18:H18)</f>
+        <f t="shared" si="0"/>
         <v>0.76595000000000002</v>
       </c>
       <c r="K18" s="13"/>
@@ -3290,7 +3290,7 @@
         <v>0.76406249999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>2.1</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>0.77190000000000003</v>
       </c>
       <c r="I19" s="12">
-        <f>AVERAGE(G19:H19)</f>
+        <f t="shared" si="0"/>
         <v>0.78034999999999999</v>
       </c>
       <c r="K19" s="13"/>
@@ -3321,7 +3321,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>2.2000000000000002</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>0.8256</v>
       </c>
       <c r="I20" s="12">
-        <f>AVERAGE(G20:H20)</f>
+        <f t="shared" si="0"/>
         <v>0.83810000000000007</v>
       </c>
       <c r="K20" s="13"/>
@@ -3352,7 +3352,7 @@
         <v>0.83750000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>2.2999999999999998</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>0.85620000000000007</v>
       </c>
       <c r="I21" s="12">
-        <f>AVERAGE(G21:H21)</f>
+        <f t="shared" si="0"/>
         <v>0.86499999999999999</v>
       </c>
       <c r="K21" s="13"/>
@@ -3383,7 +3383,7 @@
         <v>0.86468750000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>2.4</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>0.86060000000000003</v>
       </c>
       <c r="I22" s="12">
-        <f>AVERAGE(G22:H22)</f>
+        <f t="shared" si="0"/>
         <v>0.86280000000000001</v>
       </c>
       <c r="K22" s="13"/>
@@ -3414,7 +3414,7 @@
         <v>0.8621875</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>2.5</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>0.86</v>
       </c>
       <c r="I23" s="12">
-        <f>AVERAGE(G23:H23)</f>
+        <f t="shared" si="0"/>
         <v>0.87095</v>
       </c>
       <c r="K23" s="13"/>
@@ -3445,7 +3445,7 @@
         <v>0.87093750000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="13"/>
@@ -3459,7 +3459,7 @@
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="13"/>
@@ -3473,7 +3473,7 @@
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="13"/>
@@ -3487,7 +3487,7 @@
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="13"/>
@@ -3501,7 +3501,7 @@
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="13"/>
@@ -3515,7 +3515,7 @@
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="13"/>
@@ -3529,7 +3529,7 @@
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="13"/>

</xml_diff>